<commit_message>
refaktor from start to inside-specs
</commit_message>
<xml_diff>
--- a/other/dane pacjentow z artykulu.xlsx
+++ b/other/dane pacjentow z artykulu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dawid\Documents\GitHub\EngineeringProject git\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DDE74C-55C3-42D4-9ECB-1A45D70434D1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987C7B24-D468-4103-89EC-CFC91F01A80F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -537,7 +538,7 @@
   <dimension ref="A1:Z167"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A139" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="N148" sqref="N148"/>
+      <selection activeCell="N161" sqref="N161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>